<commit_message>
Redesign log format to include header for custom attributes names
</commit_message>
<xml_diff>
--- a/log_collector/resource/xlsx/sample_data.xlsx
+++ b/log_collector/resource/xlsx/sample_data.xlsx
@@ -20,7 +20,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <si>
+    <t xml:space="preserve">id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extraFieldA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">extraFieldB</t>
+  </si>
   <si>
     <t xml:space="preserve">actA</t>
   </si>
@@ -61,6 +73,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,10 +155,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -154,45 +167,59 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="n">
-        <v>19242</v>
+      <c r="A1" s="0" t="s">
+        <v>0</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>19243</v>
+        <v>19242</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
+        <v>19243</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
         <v>19244</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>8</v>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>